<commit_message>
t5a - FINALIZADO FDS
</commit_message>
<xml_diff>
--- a/T1B-arrefecimento.xlsx
+++ b/T1B-arrefecimento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2540744C-5571-4FB7-BB7B-7E1A0198CF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CD5A08-5C9C-440F-BE31-D8644680A874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Água" sheetId="1" r:id="rId1"/>
@@ -218,16 +218,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -237,6 +228,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -10479,7 +10479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F584"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -10493,18 +10493,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -10513,20 +10513,20 @@
       <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
@@ -21545,7 +21545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366A545B-4A9E-4D43-94FC-085353CA06C9}">
   <dimension ref="A1:M194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -21556,10 +21556,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -21597,12 +21597,12 @@
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -21614,17 +21614,17 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <f t="array" ref="E4:F6">LINEST(B92:B112,A92:A112,1,1)</f>
         <v>2.7272727272725718E-4</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>57.023376623376642</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="1"/>
@@ -21638,16 +21638,16 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>1.1688311688311024E-4</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <v>8.2123733721810102E-2</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="1"/>
@@ -21665,16 +21665,16 @@
         <v>95.7</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>0.22272727272727263</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>3.2433748657038283E-2</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="1"/>
@@ -21711,11 +21711,11 @@
         <v>93.9</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="12">
+      <c r="E8" s="12"/>
+      <c r="F8" s="9">
         <f>AVERAGE(B92:B112)</f>
         <v>57.214285714285722</v>
       </c>
@@ -21736,7 +21736,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -21755,7 +21755,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -21774,7 +21774,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -21793,7 +21793,7 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="11"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -21812,7 +21812,7 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="11"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -21831,7 +21831,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="11"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -21850,7 +21850,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="11"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -21869,7 +21869,7 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="8"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -21888,7 +21888,7 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="11"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -21907,7 +21907,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -21926,7 +21926,7 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="11"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -21945,7 +21945,7 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="11"/>
+      <c r="E20" s="8"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -21964,7 +21964,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="11"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -21983,7 +21983,7 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="11"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -22002,7 +22002,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="11"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -22021,7 +22021,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="11"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -22040,7 +22040,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="11"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -22059,7 +22059,7 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="11"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -22078,7 +22078,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="11"/>
+      <c r="E27" s="8"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -22097,7 +22097,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="11"/>
+      <c r="E28" s="8"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -22116,7 +22116,7 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="11"/>
+      <c r="E29" s="8"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>

</xml_diff>